<commit_message>
done cost/cal_cost.py v3.1 cost/cal_cost_dept.py v1.0 @office
Signed-off-by: socrates77 <zhwenrong@sina.com>
</commit_message>
<xml_diff>
--- a/cost/工时比例.xlsx
+++ b/cost/工时比例.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="198">
   <si>
     <t>序号</t>
   </si>
@@ -671,6 +671,10 @@
     <t>研发</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t>南京</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -911,7 +915,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1078,6 +1082,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1475,49 +1482,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="59" t="s">
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="60" t="s">
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="57" t="s">
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="58" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="9" t="s">
         <v>8</v>
       </c>
@@ -1566,7 +1573,7 @@
       <c r="T2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="58"/>
+      <c r="U2" s="59"/>
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="4">
@@ -4440,58 +4447,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="59" t="s">
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="59" t="s">
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="62"/>
       <c r="X1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="Y1" s="57" t="s">
+      <c r="Y1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="57" t="s">
+      <c r="Z1" s="58" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:26">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="12" t="s">
         <v>101</v>
       </c>
@@ -4552,8 +4559,8 @@
       <c r="X2" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="Y2" s="58"/>
-      <c r="Z2" s="58"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="4">
@@ -9216,60 +9223,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="59" t="s">
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="59" t="s">
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="62"/>
       <c r="Z1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="AA1" s="57" t="s">
+      <c r="AA1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="57" t="s">
+      <c r="AB1" s="58" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:28">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="29" t="s">
         <v>101</v>
       </c>
@@ -9336,8 +9343,8 @@
       <c r="Z2" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="AA2" s="58"/>
-      <c r="AB2" s="58"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="59"/>
     </row>
     <row r="3" spans="1:28">
       <c r="A3" s="4">
@@ -14252,60 +14259,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="59" t="s">
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="59" t="s">
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="62"/>
       <c r="Z1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="AA1" s="57" t="s">
+      <c r="AA1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="57" t="s">
+      <c r="AB1" s="58" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:28">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="33" t="s">
         <v>101</v>
       </c>
@@ -14372,8 +14379,8 @@
       <c r="Z2" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="AA2" s="58"/>
-      <c r="AB2" s="58"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="59"/>
     </row>
     <row r="3" spans="1:28">
       <c r="A3" s="4">
@@ -19303,7 +19310,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -19328,63 +19335,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="59" t="s">
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="59" t="s">
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="62"/>
       <c r="Z1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="AA1" s="57" t="s">
+      <c r="AA1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="57" t="s">
+      <c r="AB1" s="58" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:28">
-      <c r="A2" s="62"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="44" t="s">
         <v>180</v>
       </c>
@@ -19448,15 +19455,15 @@
       <c r="Z2" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="AA2" s="58"/>
-      <c r="AB2" s="58"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="59"/>
     </row>
     <row r="3" spans="1:28">
-      <c r="A3" s="58"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
       <c r="F3" s="56" t="s">
         <v>192</v>
       </c>
@@ -19467,10 +19474,10 @@
         <v>194</v>
       </c>
       <c r="I3" s="56" t="s">
-        <v>194</v>
-      </c>
-      <c r="J3" s="56" t="s">
-        <v>194</v>
+        <v>197</v>
+      </c>
+      <c r="J3" s="57" t="s">
+        <v>197</v>
       </c>
       <c r="K3" s="56" t="s">
         <v>194</v>
@@ -19488,7 +19495,7 @@
         <v>194</v>
       </c>
       <c r="P3" s="56" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="Q3" s="56" t="s">
         <v>194</v>
@@ -24397,16 +24404,16 @@
     <filterColumn colId="23" showButton="0"/>
   </autoFilter>
   <mergeCells count="10">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="D1:D3"/>
     <mergeCell ref="Q1:Y1"/>
     <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="F1:L1"/>
     <mergeCell ref="M1:P1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="D1:D3"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>